<commit_message>
Ahora funciona, hay que cambiar la clase Ui_Caja
</commit_message>
<xml_diff>
--- a/datos.xlsx
+++ b/datos.xlsx
@@ -434,7 +434,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -579,6 +579,21 @@
       </c>
       <c r="C10" t="n">
         <v>123456789</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>1234</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>migue</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>123456789</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -657,7 +672,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -970,6 +985,40 @@
       <c r="H9" t="inlineStr">
         <is>
           <t>31/05/2024 16:31</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>REF123</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>1234567890123</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Marca A</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>10</v>
+      </c>
+      <c r="E10" t="n">
+        <v>20</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" t="b">
+        <v>0</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>31/05/2024 23:09</t>
         </is>
       </c>
     </row>
@@ -1039,7 +1088,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1366,6 +1415,40 @@
         <v>3221</v>
       </c>
       <c r="H9" t="inlineStr">
+        <is>
+          <t>efectivo</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>123</v>
+      </c>
+      <c r="B10" t="n">
+        <v>1234</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>migue</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Shampoo</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>31/05/2024 23:09</t>
+        </is>
+      </c>
+      <c r="F10" t="n">
+        <v>12</v>
+      </c>
+      <c r="G10" t="n">
+        <v>3221</v>
+      </c>
+      <c r="H10" t="inlineStr">
         <is>
           <t>efectivo</t>
         </is>
@@ -1494,7 +1577,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1720,6 +1803,29 @@
         </is>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>12</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>mgiue</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>345</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>31/05/2024 23:09</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>28/05/2024 14:30</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -1731,7 +1837,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2001,6 +2107,33 @@
         <v>1</v>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>1234</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>migue</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>31/05/2024 23:09</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>3221</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" t="n">
+        <v>3221</v>
+      </c>
+      <c r="G10" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -2012,7 +2145,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2192,6 +2325,22 @@
         <v>2</v>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>2</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>12345</v>
+      </c>
+      <c r="D11" t="n">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
diseño de reportes terminado (quedo con fallas menores), falta conectar con API
</commit_message>
<xml_diff>
--- a/datos.xlsx
+++ b/datos.xlsx
@@ -434,7 +434,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -518,15 +518,15 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>123124</v>
+        <v>1234</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>pedro</t>
+          <t>migue</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>54321</v>
+        <v>123456789</v>
       </c>
     </row>
     <row r="7">
@@ -578,6 +578,32 @@
         </is>
       </c>
       <c r="C10" t="n">
+        <v>123456789</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>1234</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>migue</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>123456789</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>1234</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>migue</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
         <v>123456789</v>
       </c>
     </row>
@@ -657,7 +683,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -745,7 +771,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>31/05/2024 16:15</t>
+          <t>01/06/2024 03:17</t>
         </is>
       </c>
     </row>
@@ -777,7 +803,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>31/05/2024 16:16</t>
+          <t>01/06/2024 03:19</t>
         </is>
       </c>
     </row>
@@ -809,7 +835,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>31/05/2024 16:18</t>
+          <t>01/06/2024 03:23</t>
         </is>
       </c>
     </row>
@@ -841,7 +867,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>31/05/2024 16:20</t>
+          <t>01/06/2024 03:24</t>
         </is>
       </c>
     </row>
@@ -873,7 +899,7 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>31/05/2024 16:21</t>
+          <t>01/06/2024 03:25</t>
         </is>
       </c>
     </row>
@@ -905,7 +931,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>31/05/2024 16:26</t>
+          <t>01/06/2024 03:26</t>
         </is>
       </c>
     </row>
@@ -937,7 +963,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>31/05/2024 16:30</t>
+          <t>01/06/2024 03:29</t>
         </is>
       </c>
     </row>
@@ -969,7 +995,103 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>31/05/2024 16:31</t>
+          <t>01/06/2024 03:33</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>REF123</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>1234567890123</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Marca A</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>10</v>
+      </c>
+      <c r="E10" t="n">
+        <v>20</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" t="b">
+        <v>0</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>01/06/2024 03:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>REF123</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>1234567890123</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Marca A</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>10</v>
+      </c>
+      <c r="E11" t="n">
+        <v>20</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" t="b">
+        <v>0</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>01/06/2024 03:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>REF123</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>1234567890123</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Marca A</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>10</v>
+      </c>
+      <c r="E12" t="n">
+        <v>20</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" t="b">
+        <v>0</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>01/06/2024 03:39</t>
         </is>
       </c>
     </row>
@@ -1039,7 +1161,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1118,7 +1240,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>31/05/2024 16:15</t>
+          <t>01/06/2024 03:17</t>
         </is>
       </c>
       <c r="F2" t="n">
@@ -1152,7 +1274,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>31/05/2024 16:16</t>
+          <t>01/06/2024 03:19</t>
         </is>
       </c>
       <c r="F3" t="n">
@@ -1186,7 +1308,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>31/05/2024 16:18</t>
+          <t>01/06/2024 03:23</t>
         </is>
       </c>
       <c r="F4" t="n">
@@ -1220,7 +1342,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>31/05/2024 16:20</t>
+          <t>01/06/2024 03:24</t>
         </is>
       </c>
       <c r="F5" t="n">
@@ -1254,7 +1376,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>31/05/2024 16:21</t>
+          <t>01/06/2024 03:25</t>
         </is>
       </c>
       <c r="F6" t="n">
@@ -1288,7 +1410,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>31/05/2024 16:26</t>
+          <t>01/06/2024 03:26</t>
         </is>
       </c>
       <c r="F7" t="n">
@@ -1322,7 +1444,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>31/05/2024 16:30</t>
+          <t>01/06/2024 03:29</t>
         </is>
       </c>
       <c r="F8" t="n">
@@ -1356,7 +1478,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>31/05/2024 16:31</t>
+          <t>01/06/2024 03:33</t>
         </is>
       </c>
       <c r="F9" t="n">
@@ -1366,6 +1488,108 @@
         <v>3221</v>
       </c>
       <c r="H9" t="inlineStr">
+        <is>
+          <t>efectivo</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>123</v>
+      </c>
+      <c r="B10" t="n">
+        <v>1234</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>migue</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Shampoo</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>01/06/2024 03:36</t>
+        </is>
+      </c>
+      <c r="F10" t="n">
+        <v>12</v>
+      </c>
+      <c r="G10" t="n">
+        <v>3221</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>efectivo</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>123</v>
+      </c>
+      <c r="B11" t="n">
+        <v>1234</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>migue</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Shampoo</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>01/06/2024 03:38</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
+        <v>12</v>
+      </c>
+      <c r="G11" t="n">
+        <v>3221</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>efectivo</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>123</v>
+      </c>
+      <c r="B12" t="n">
+        <v>1234</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>migue</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Shampoo</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>01/06/2024 03:39</t>
+        </is>
+      </c>
+      <c r="F12" t="n">
+        <v>12</v>
+      </c>
+      <c r="G12" t="n">
+        <v>3221</v>
+      </c>
+      <c r="H12" t="inlineStr">
         <is>
           <t>efectivo</t>
         </is>
@@ -1494,7 +1718,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1550,7 +1774,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>31/05/2024 16:15</t>
+          <t>01/06/2024 03:17</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -1573,7 +1797,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>31/05/2024 16:16</t>
+          <t>01/06/2024 03:19</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -1596,7 +1820,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>31/05/2024 16:18</t>
+          <t>01/06/2024 03:23</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -1619,7 +1843,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>31/05/2024 16:20</t>
+          <t>01/06/2024 03:24</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -1642,7 +1866,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>31/05/2024 16:21</t>
+          <t>01/06/2024 03:25</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -1665,7 +1889,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>31/05/2024 16:26</t>
+          <t>01/06/2024 03:26</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -1688,7 +1912,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>31/05/2024 16:30</t>
+          <t>01/06/2024 03:29</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -1711,10 +1935,79 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>31/05/2024 16:31</t>
+          <t>01/06/2024 03:33</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
+        <is>
+          <t>28/05/2024 14:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>12</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>mgiue</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>345</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>01/06/2024 03:36</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>28/05/2024 14:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>12</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>mgiue</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>345</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>01/06/2024 03:38</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>28/05/2024 14:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>12</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>mgiue</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>345</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>01/06/2024 03:39</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
         <is>
           <t>28/05/2024 14:30</t>
         </is>
@@ -1731,7 +2024,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1796,7 +2089,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>31/05/2024 16:15</t>
+          <t>01/06/2024 03:17</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -1823,7 +2116,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>31/05/2024 16:16</t>
+          <t>01/06/2024 03:19</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -1850,7 +2143,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>31/05/2024 16:18</t>
+          <t>01/06/2024 03:23</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -1877,7 +2170,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>31/05/2024 16:20</t>
+          <t>01/06/2024 03:24</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -1904,7 +2197,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>31/05/2024 16:21</t>
+          <t>01/06/2024 03:25</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -1931,7 +2224,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>31/05/2024 16:26</t>
+          <t>01/06/2024 03:26</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -1958,7 +2251,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>31/05/2024 16:30</t>
+          <t>01/06/2024 03:29</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -1985,7 +2278,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>31/05/2024 16:31</t>
+          <t>01/06/2024 03:33</t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -1998,6 +2291,87 @@
         <v>3221</v>
       </c>
       <c r="G9" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>1234</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>migue</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>01/06/2024 03:36</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>3221</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" t="n">
+        <v>3221</v>
+      </c>
+      <c r="G10" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>1234</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>migue</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>01/06/2024 03:38</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>3221</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" t="n">
+        <v>3221</v>
+      </c>
+      <c r="G11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>1234</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>migue</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>01/06/2024 03:39</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>3221</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" t="n">
+        <v>3221</v>
+      </c>
+      <c r="G12" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2012,7 +2386,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2192,6 +2566,54 @@
         <v>2</v>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>2</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>12345</v>
+      </c>
+      <c r="D11" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>2</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>12345</v>
+      </c>
+      <c r="D12" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>2</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>12345</v>
+      </c>
+      <c r="D13" t="n">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>